<commit_message>
summarise by grouping variable
</commit_message>
<xml_diff>
--- a/input-data/lseg_columns_needed.xlsx
+++ b/input-data/lseg_columns_needed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucbvlm0_ucl_ac_uk/Documents/Documents/programming/main-projects/amazon-footprint/input-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="706" documentId="8_{59694D10-1ADE-A449-AC98-835B8DC94CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5385B9CC-AAA1-7648-A1A1-E5198D06BE96}"/>
+  <xr:revisionPtr revIDLastSave="707" documentId="8_{59694D10-1ADE-A449-AC98-835B8DC94CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B7031FD-75A4-B74F-AC2F-5B68FD2EA306}"/>
   <bookViews>
     <workbookView xWindow="4600" yWindow="1220" windowWidth="18380" windowHeight="16480" xr2:uid="{AD20F702-6B9F-7F4A-9CFC-34D2E60F3FF2}"/>
   </bookViews>
@@ -1468,12 +1468,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E580FEAB-E6CC-8840-B63D-FCC67799A767}">
   <dimension ref="A1:G198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="A199" sqref="A199:A202"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153:C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
@@ -4795,26 +4796,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="193858b9-a7e5-46a0-a17e-3020908dcb20">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="74939e57-9d5a-4a0e-92b8-734534a31947" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100782D128FB6981541A51099910CFC1E4B" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f74102cfec586183eca87f50d115a912">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="193858b9-a7e5-46a0-a17e-3020908dcb20" xmlns:ns3="74939e57-9d5a-4a0e-92b8-734534a31947" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="80a57a212c8dac7c54b70a8786012a0b" ns2:_="" ns3:_="">
     <xsd:import namespace="193858b9-a7e5-46a0-a17e-3020908dcb20"/>
@@ -5063,32 +5044,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F3FA12-1D2A-49BC-ACD8-7A41D6FBC181}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="74939e57-9d5a-4a0e-92b8-734534a31947"/>
-    <ds:schemaRef ds:uri="193858b9-a7e5-46a0-a17e-3020908dcb20"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{440E0154-4747-4FA3-8651-122E7C61EF0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="193858b9-a7e5-46a0-a17e-3020908dcb20">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="74939e57-9d5a-4a0e-92b8-734534a31947" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{642F7E26-E2A6-4CAB-8C0E-88FD4AF632AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5107,6 +5083,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{440E0154-4747-4FA3-8651-122E7C61EF0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9F3FA12-1D2A-49BC-ACD8-7A41D6FBC181}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="74939e57-9d5a-4a0e-92b8-734534a31947"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="193858b9-a7e5-46a0-a17e-3020908dcb20"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{1faf88fe-a998-4c5b-93c9-210a11d9a5c2}" enabled="0" method="" siteId="{1faf88fe-a998-4c5b-93c9-210a11d9a5c2}" removed="1"/>

</xml_diff>